<commit_message>
add runmg tests and fixed small errors
</commit_message>
<xml_diff>
--- a/test/GeneratorTest_case14inconsistente.xlsx
+++ b/test/GeneratorTest_case14inconsistente.xlsx
@@ -702,7 +702,7 @@
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1397,7 +1397,7 @@
   <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:L13"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1486,31 +1486,31 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D3">
-        <v>13.119947374380338</v>
+        <v>1</v>
       </c>
       <c r="E3">
-        <v>1.0000000000000001E-5</v>
+        <v>1</v>
       </c>
       <c r="F3">
         <v>1</v>
       </c>
       <c r="G3">
-        <v>1.4935811303782169</v>
+        <v>1</v>
       </c>
       <c r="H3">
-        <v>1.0000000000000001E-5</v>
+        <v>1</v>
       </c>
       <c r="I3">
         <v>1</v>
       </c>
       <c r="J3">
-        <v>13.12120804346363</v>
+        <v>1</v>
       </c>
       <c r="K3">
-        <v>1.4924926783026791</v>
+        <v>1</v>
       </c>
       <c r="L3">
         <v>1</v>
@@ -1542,7 +1542,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="I4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J4">
         <v>11.405350787245393</v>
@@ -1647,7 +1647,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="F7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G7">
         <v>0.39935239778069975</v>
@@ -1694,7 +1694,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="I8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J8">
         <v>0.95314566372372822</v>
@@ -1761,7 +1761,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="F10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G10">
         <v>3.9629128531944807E-2</v>
@@ -1905,8 +1905,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2042,7 +2042,7 @@
         <v>1E-4</v>
       </c>
       <c r="I4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J4">
         <v>0.75510381824287731</v>
@@ -2068,7 +2068,7 @@
         <v>1E-4</v>
       </c>
       <c r="F5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G5">
         <v>4.2619249932304266E-2</v>
@@ -2112,7 +2112,7 @@
         <v>1E-4</v>
       </c>
       <c r="I6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J6">
         <v>0.56131495938735865</v>
@@ -2173,7 +2173,7 @@
         <v>1E-4</v>
       </c>
       <c r="F8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G8">
         <v>3.757456160128398E-2</v>
@@ -2252,7 +2252,7 @@
         <v>1E-4</v>
       </c>
       <c r="I10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J10">
         <v>0.28074175915785449</v>
@@ -2348,7 +2348,7 @@
         <v>1E-4</v>
       </c>
       <c r="F13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G13">
         <v>1.5625054525863706E-2</v>
@@ -2427,7 +2427,7 @@
         <v>1E-4</v>
       </c>
       <c r="I15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J15">
         <v>-0.54454838106704917</v>
@@ -2593,7 +2593,7 @@
         <v>1E-4</v>
       </c>
       <c r="F20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G20">
         <v>1.7714324523559061E-3</v>
@@ -2733,7 +2733,7 @@
         <v>1E-4</v>
       </c>
       <c r="F24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G24">
         <v>-1.5973947303893968E-2</v>
@@ -2796,7 +2796,7 @@
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:XFD11"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2870,7 +2870,7 @@
         <v>1E-4</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3">
         <v>-0.17019450861146554</v>
@@ -2908,7 +2908,7 @@
         <v>1E-4</v>
       </c>
       <c r="G4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H4">
         <v>0.18300000000266339</v>
@@ -2928,7 +2928,7 @@
         <v>1E-4</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5">
         <v>4.9301984316690674E-2</v>
@@ -2995,7 +2995,7 @@
         <v>1E-4</v>
       </c>
       <c r="G7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H7">
         <v>-7.5999999979886865E-2</v>
@@ -3044,7 +3044,7 @@
         <v>1E-4</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E9">
         <v>-6.0184743626494536E-2</v>
@@ -3130,7 +3130,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3180,7 +3180,7 @@
         <v>1E-4</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3">
         <v>1.06</v>
@@ -3231,7 +3231,7 @@
         <v>1E-4</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6">
         <v>1.0176708536972445</v>
@@ -3248,7 +3248,7 @@
         <v>1E-4</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E7">
         <v>1.019513859822472</v>
@@ -3299,7 +3299,7 @@
         <v>1E-4</v>
       </c>
       <c r="D10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E10">
         <v>1.0569065185415225</v>

</xml_diff>